<commit_message>
- Simplified solnpool.py by setting pool mode to 2 - Updates tests cases with some new tests and some TODOs
</commit_message>
<xml_diff>
--- a/pyomo/contrib/alternative_solutions/tests/test_case.xlsx
+++ b/pyomo/contrib/alternative_solutions/tests/test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlgearh\Desktop\Code\CI-MOR\pyomo\pyomo\contrib\alternative_solutions\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33D6E82-9819-48A7-9110-3C92CE73F4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799A77B4-9F9A-45E8-A39A-E02F910A0015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="0" windowWidth="27000" windowHeight="15450" xr2:uid="{363FAE57-B912-4644-9513-01EF5EFD5CFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{363FAE57-B912-4644-9513-01EF5EFD5CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4916ABC8-9B79-4BDB-9EAC-F7A35FEBA08A}">
-  <dimension ref="C4:S12"/>
+  <dimension ref="C4:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="S11" sqref="S11:S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,11 +687,6 @@
         <v>-0.78947368421052611</v>
       </c>
     </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="S12">
-        <v>2.3076923076923075</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Added code to enumerate the discrete feasiable points for the diamond problem and found the extreme points and domain for a particular objective constraint
</commit_message>
<xml_diff>
--- a/pyomo/contrib/alternative_solutions/tests/test_case.xlsx
+++ b/pyomo/contrib/alternative_solutions/tests/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlgearh\Desktop\Code\CI-MOR\pyomo\pyomo\contrib\alternative_solutions\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799A77B4-9F9A-45E8-A39A-E02F910A0015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383A2212-01AB-4AFD-ABC8-86CC3EAAEBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{363FAE57-B912-4644-9513-01EF5EFD5CFB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>x</t>
   </si>
@@ -64,14 +64,25 @@
   </si>
   <si>
     <t>b2</t>
+  </si>
+  <si>
+    <t>Objective</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,15 +427,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4916ABC8-9B79-4BDB-9EAC-F7A35FEBA08A}">
-  <dimension ref="C4:S8"/>
+  <dimension ref="C4:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11:S13"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -466,8 +478,11 @@
       <c r="S4" t="s">
         <v>1</v>
       </c>
+      <c r="T4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1</v>
       </c>
@@ -521,8 +536,12 @@
         <f>R5*N5+O5</f>
         <v>-4.5901639344262293</v>
       </c>
+      <c r="T5">
+        <f>R5+S5</f>
+        <v>-3.8524590163934427</v>
+      </c>
     </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>2</v>
       </c>
@@ -576,8 +595,12 @@
         <f t="shared" ref="S6:S8" si="7">R6*N6+O6</f>
         <v>0.6956521739130439</v>
       </c>
+      <c r="T6">
+        <f t="shared" ref="T6:T8" si="8">R6+S6</f>
+        <v>-5.1739130434782608</v>
+      </c>
     </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
@@ -631,8 +654,12 @@
         <f t="shared" si="7"/>
         <v>2.3076923076923075</v>
       </c>
+      <c r="T7">
+        <f t="shared" si="8"/>
+        <v>3.6923076923076921</v>
+      </c>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>4</v>
       </c>
@@ -686,8 +713,13 @@
         <f t="shared" si="7"/>
         <v>-0.78947368421052611</v>
       </c>
+      <c r="T8" s="1">
+        <f t="shared" si="8"/>
+        <v>6.7894736842105257</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>